<commit_message>
fixed Advanced Search Engine
</commit_message>
<xml_diff>
--- a/data/ANOR_suppl_mat.xlsx
+++ b/data/ANOR_suppl_mat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manju\Dropbox\ANOR_Paper\optimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manju\Dropbox\ANOR_Paper\ANOR_Revised_1019\ANOR1028\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C30B409-B98A-465A-A3FA-886B6BB211BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1977411B-FF62-49AE-85B9-BDE060502197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{96C00013-20FD-4176-8B80-7A1DAAAC34AF}"/>
   </bookViews>
@@ -16,13 +16,13 @@
     <sheet name="Neuron variables" sheetId="31" r:id="rId1"/>
     <sheet name="Equations" sheetId="25" r:id="rId2"/>
     <sheet name="Results" sheetId="49" r:id="rId3"/>
-    <sheet name="validation_table" sheetId="53" r:id="rId4"/>
+    <sheet name="stereology_visualization" sheetId="53" r:id="rId4"/>
     <sheet name="Matrix" sheetId="51" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">validation_table!$A$2:$A$30</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">validation_table!$C$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">validation_table!$C$2:$C$30</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">stereology_visualization!$A$2:$A$30</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">stereology_visualization!$C$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">stereology_visualization!$C$2:$C$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="315">
   <si>
     <t>X1</t>
   </si>
@@ -423,12 +423,6 @@
     <t>Method</t>
   </si>
   <si>
-    <t>Original equation</t>
-  </si>
-  <si>
-    <t>(x19+x20) = 2*(x10+x18)</t>
-  </si>
-  <si>
     <t>(x19+x20)/(2*x10 + 2*x18) - 1 = 0</t>
   </si>
   <si>
@@ -459,9 +453,6 @@
     <t>(x13+x14+x21)/x17 = 6/11</t>
   </si>
   <si>
-    <t>x17 = x22+x15</t>
-  </si>
-  <si>
     <t>(x10+x18)/x3 = 169/64</t>
   </si>
   <si>
@@ -501,9 +492,6 @@
     <t>equation converted as per reviewer's suggestion</t>
   </si>
   <si>
-    <t>weights</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -982,6 +970,21 @@
   </si>
   <si>
     <t>Lister et al. 2006</t>
+  </si>
+  <si>
+    <t>(x17)/(x22+x15) = 1</t>
+  </si>
+  <si>
+    <t>(x19+x20)/(2*(x10+x18)) = 1</t>
+  </si>
+  <si>
+    <t>Percent-error equation</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t>Measurement equation</t>
   </si>
 </sst>
 </file>
@@ -2748,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08344D76-65AF-41DB-B550-B70AE27E37F3}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="80" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15.6"/>
@@ -2764,13 +2767,13 @@
   <sheetData>
     <row r="1" spans="1:6" s="50" customFormat="1" ht="45" customHeight="1">
       <c r="A1" s="62" t="s">
-        <v>153</v>
+        <v>313</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>152</v>
+        <v>312</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>127</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>45</v>
@@ -2779,7 +2782,7 @@
         <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.2">
@@ -2787,10 +2790,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>128</v>
+        <v>311</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>55</v>
@@ -2805,10 +2808,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>91</v>
@@ -2825,10 +2828,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>95</v>
@@ -2845,10 +2848,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>92</v>
@@ -2865,10 +2868,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>93</v>
@@ -2885,10 +2888,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>94</v>
@@ -2905,10 +2908,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>96</v>
@@ -2925,10 +2928,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>97</v>
@@ -2945,10 +2948,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>98</v>
@@ -2965,10 +2968,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>99</v>
@@ -2985,10 +2988,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>100</v>
@@ -3005,10 +3008,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>117</v>
@@ -3025,10 +3028,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>139</v>
+        <v>310</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>118</v>
@@ -3045,10 +3048,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>119</v>
@@ -3065,10 +3068,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C16" s="45" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>77</v>
@@ -3085,10 +3088,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>125</v>
@@ -3105,10 +3108,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="45" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>58</v>
@@ -3125,10 +3128,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>59</v>
@@ -3145,10 +3148,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>60</v>
@@ -3165,10 +3168,10 @@
         <v>10</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>61</v>
@@ -3185,10 +3188,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>62</v>
@@ -3205,10 +3208,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>120</v>
@@ -3223,16 +3226,16 @@
         <v>10</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C24" s="45" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>66</v>
@@ -3243,10 +3246,10 @@
         <v>10</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>121</v>
@@ -3263,10 +3266,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C26" s="45" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>122</v>
@@ -3283,16 +3286,16 @@
         <v>10</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>124</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F27" s="53">
         <f>(1032255/2)/0.41</f>
@@ -3304,16 +3307,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>67</v>
@@ -3324,16 +3327,16 @@
         <v>10</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C29" s="45" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="46.8">
@@ -3341,16 +3344,16 @@
         <v>10</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="46.8">
@@ -3358,16 +3361,16 @@
         <v>10</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="46.8">
@@ -3375,16 +3378,16 @@
         <v>10</v>
       </c>
       <c r="B32" s="45" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="46.8">
@@ -3392,16 +3395,16 @@
         <v>10</v>
       </c>
       <c r="B33" s="45" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="46.8">
@@ -3409,16 +3412,16 @@
         <v>10</v>
       </c>
       <c r="B34" s="45" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C34" s="45" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="46.8">
@@ -3426,16 +3429,16 @@
         <v>10</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="46.8">
@@ -3443,16 +3446,16 @@
         <v>10</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C36" s="45" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="46.8">
@@ -3460,16 +3463,16 @@
         <v>1</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C37" s="45" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="31.2">
@@ -3477,16 +3480,16 @@
         <v>10</v>
       </c>
       <c r="B38" s="45" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C38" s="45" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="31.2">
@@ -3494,16 +3497,16 @@
         <v>10</v>
       </c>
       <c r="B39" s="45" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C39" s="45" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="31.2">
@@ -3511,16 +3514,16 @@
         <v>10</v>
       </c>
       <c r="B40" s="45" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C40" s="45" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="31.2">
@@ -3528,16 +3531,16 @@
         <v>10</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="31.2">
@@ -3545,16 +3548,16 @@
         <v>10</v>
       </c>
       <c r="B42" s="45" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C42" s="45" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="31.2">
@@ -3562,16 +3565,16 @@
         <v>10</v>
       </c>
       <c r="B43" s="45" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C43" s="45" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="31.2">
@@ -3579,16 +3582,16 @@
         <v>10</v>
       </c>
       <c r="B44" s="45" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="46.8">
@@ -3596,16 +3599,16 @@
         <v>1</v>
       </c>
       <c r="B45" s="45" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="46.8">
@@ -3613,16 +3616,16 @@
         <v>1</v>
       </c>
       <c r="B46" s="45" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C46" s="45" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="56" customFormat="1" ht="43.2">
@@ -3630,19 +3633,19 @@
         <v>10</v>
       </c>
       <c r="B47" s="45" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C47" s="45" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="56" customFormat="1" ht="31.2">
@@ -3650,19 +3653,19 @@
         <v>10</v>
       </c>
       <c r="B48" s="45" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C48" s="45" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="56" customFormat="1" ht="46.8">
@@ -3670,19 +3673,19 @@
         <v>10</v>
       </c>
       <c r="B49" s="45" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="31.2">
@@ -3690,19 +3693,19 @@
         <v>10</v>
       </c>
       <c r="B50" s="45" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C50" s="45" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="31.2">
@@ -3710,19 +3713,19 @@
         <v>10</v>
       </c>
       <c r="B51" s="45" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C51" s="45" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3763,10 +3766,10 @@
         <v>126</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>22</v>
@@ -3857,7 +3860,7 @@
     </row>
     <row r="2" spans="1:45" s="58" customFormat="1" ht="15.6">
       <c r="A2" s="58" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B2" s="59">
         <v>64.2</v>
@@ -3935,7 +3938,7 @@
     </row>
     <row r="3" spans="1:45" s="49" customFormat="1" ht="16.5" customHeight="1">
       <c r="A3" s="29" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B3" s="30">
         <v>23.470556025788259</v>
@@ -4013,7 +4016,7 @@
     </row>
     <row r="4" spans="1:45" s="32" customFormat="1" ht="15.6">
       <c r="A4" s="31" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B4" s="30">
         <v>23.468344253437859</v>
@@ -4091,7 +4094,7 @@
     </row>
     <row r="5" spans="1:45" s="34" customFormat="1" ht="15.6">
       <c r="A5" s="33" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B5" s="74">
         <v>42.045178597882277</v>
@@ -4169,7 +4172,7 @@
     </row>
     <row r="6" spans="1:45" s="34" customFormat="1" ht="15.6">
       <c r="A6" s="34" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B6" s="74">
         <v>48.207161544542295</v>
@@ -4247,7 +4250,7 @@
     </row>
     <row r="7" spans="1:45" s="37" customFormat="1" ht="15.6">
       <c r="A7" s="35" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B7" s="57">
         <v>161.93651992581795</v>
@@ -4325,7 +4328,7 @@
     </row>
     <row r="8" spans="1:45" s="37" customFormat="1" ht="15.6">
       <c r="A8" s="38" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B8" s="57">
         <v>161.93651992581795</v>
@@ -4449,7 +4452,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4465,434 +4468,434 @@
   <sheetData>
     <row r="1" spans="1:14" ht="14.7" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.7" thickBot="1">
       <c r="A2" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C2" s="16">
         <v>341583</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14" ht="14.7" thickBot="1">
       <c r="A3" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C3" s="16">
         <v>147050</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:14" s="67" customFormat="1" ht="14.7" thickBot="1">
       <c r="A4" s="63" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B4" s="64" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C4" s="65">
         <v>158845.52906662007</v>
       </c>
       <c r="D4" s="66" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N4" s="68"/>
     </row>
     <row r="5" spans="1:14" ht="14.7" thickBot="1">
       <c r="A5" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C5" s="16">
         <v>378459</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="N5" s="22"/>
     </row>
     <row r="6" spans="1:14" ht="14.7" thickBot="1">
       <c r="A6" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C6" s="16">
         <v>1200000</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N6" s="22"/>
     </row>
     <row r="7" spans="1:14" ht="14.7" thickBot="1">
       <c r="A7" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C7" s="16">
         <v>1080000</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N7" s="22"/>
     </row>
     <row r="8" spans="1:14" ht="14.7" thickBot="1">
       <c r="A8" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C8" s="16">
         <v>1065000</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N8" s="22"/>
     </row>
     <row r="9" spans="1:14" ht="14.7" thickBot="1">
       <c r="A9" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C9" s="16">
         <v>1200000</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N9" s="22"/>
     </row>
     <row r="10" spans="1:14" ht="14.7" thickBot="1">
       <c r="A10" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C10" s="16">
         <v>1180000</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N10" s="22"/>
     </row>
     <row r="11" spans="1:14" ht="25.2" customHeight="1" thickBot="1">
       <c r="A11" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C11" s="16">
         <v>969900</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N11" s="22"/>
     </row>
     <row r="12" spans="1:14" ht="14.7" thickBot="1">
       <c r="A12" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C12" s="16">
         <v>1200000</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N12" s="22"/>
     </row>
     <row r="13" spans="1:14" ht="14.7" thickBot="1">
       <c r="A13" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C13" s="16">
         <v>1172290</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N13" s="22"/>
     </row>
     <row r="14" spans="1:14" ht="14.7" thickBot="1">
       <c r="A14" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C14" s="16">
         <v>1200000</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="14.7" thickBot="1">
       <c r="A15" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C15" s="16">
         <v>1756098</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="14.7" thickBot="1">
       <c r="A16" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C16" s="16">
         <v>1073171</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.7" thickBot="1">
       <c r="A17" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C17" s="16">
         <v>762663</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="67" customFormat="1" ht="14.7" thickBot="1">
       <c r="A18" s="63" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B18" s="64" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C18" s="65">
         <v>988759.02058439271</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.7" thickBot="1">
       <c r="A19" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C19" s="16">
         <v>648505</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.7" thickBot="1">
       <c r="A20" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C20" s="16">
         <v>65420</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.7" thickBot="1">
       <c r="A21" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C21" s="16">
         <v>52495</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.7" thickBot="1">
       <c r="A22" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C22" s="16">
         <v>53000</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.7" thickBot="1">
       <c r="A23" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C23" s="16">
         <v>63200</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.7" thickBot="1">
       <c r="A24" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C24" s="16">
         <v>49275</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.7" thickBot="1">
       <c r="A25" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C25" s="16">
         <v>45000</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.7" thickBot="1">
       <c r="A26" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C26" s="16">
         <v>40000</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.7" thickBot="1">
       <c r="A27" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C27" s="16">
         <v>154600</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.7" thickBot="1">
       <c r="A28" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C28" s="16">
         <v>44295</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="67" customFormat="1">
       <c r="A29" s="69" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B29" s="70" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C29" s="71">
         <v>46610.374314712186</v>
       </c>
       <c r="D29" s="72" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C30" s="48">
         <v>127550</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5007,10 +5010,10 @@
         <v>82</v>
       </c>
       <c r="X1" s="42" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -5084,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Y2" s="9">
         <v>1</v>
@@ -5161,7 +5164,7 @@
         <v>0</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="Y3" s="9">
         <v>1</v>
@@ -5238,7 +5241,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="45" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Y4" s="9">
         <v>1</v>
@@ -5315,7 +5318,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="45" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="Y5" s="9">
         <v>1</v>
@@ -5392,7 +5395,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="45" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Y6" s="9">
         <v>1</v>
@@ -5469,7 +5472,7 @@
         <v>0</v>
       </c>
       <c r="X7" s="45" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Y7" s="9">
         <v>1</v>
@@ -5546,7 +5549,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="45" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="Y8" s="9">
         <v>1</v>
@@ -5623,7 +5626,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="45" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="Y9" s="9">
         <v>1</v>
@@ -5700,7 +5703,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="45" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="Y10" s="9">
         <v>1</v>
@@ -5777,7 +5780,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="45" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Y11" s="9">
         <v>1</v>
@@ -5854,7 +5857,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="45" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Y12" s="9">
         <v>1</v>
@@ -5931,7 +5934,7 @@
         <v>0</v>
       </c>
       <c r="X13" s="45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="Y13" s="9">
         <v>1</v>
@@ -6008,7 +6011,7 @@
         <v>0</v>
       </c>
       <c r="X14" s="45" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="Y14" s="9">
         <v>1</v>
@@ -6085,7 +6088,7 @@
         <v>0</v>
       </c>
       <c r="X15" s="45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="Y15" s="9">
         <v>1</v>
@@ -6162,7 +6165,7 @@
         <v>35900</v>
       </c>
       <c r="X16" s="45" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="Y16" s="9">
         <v>1</v>
@@ -6239,7 +6242,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="45" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="Y17" s="9">
         <v>1</v>
@@ -6316,7 +6319,7 @@
         <v>0</v>
       </c>
       <c r="X18" s="45" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Y18" s="9">
         <v>1</v>
@@ -6393,7 +6396,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="45" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="Y19" s="9">
         <v>1</v>
@@ -6470,7 +6473,7 @@
         <v>748782</v>
       </c>
       <c r="X20" s="45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="Y20" s="9">
         <v>1</v>
@@ -6547,7 +6550,7 @@
         <v>762663</v>
       </c>
       <c r="X21" s="45" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="Y21" s="9">
         <v>1</v>
@@ -6624,7 +6627,7 @@
         <v>154600</v>
       </c>
       <c r="X22" s="45" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="Y22" s="9">
         <v>1</v>
@@ -6701,7 +6704,7 @@
         <v>341583</v>
       </c>
       <c r="X23" s="45" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="Y23" s="9">
         <v>1</v>
@@ -6778,7 +6781,7 @@
         <v>1080000</v>
       </c>
       <c r="X24" s="45" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="Y24" s="9">
         <v>10</v>
@@ -6855,7 +6858,7 @@
         <v>1065000</v>
       </c>
       <c r="X25" s="45" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Y25" s="9">
         <v>10</v>
@@ -6932,7 +6935,7 @@
         <v>1180000</v>
       </c>
       <c r="X26" s="45" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="Y26" s="9">
         <v>10</v>
@@ -7009,7 +7012,7 @@
         <v>969900</v>
       </c>
       <c r="X27" s="45" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="Y27" s="9">
         <v>10</v>
@@ -7086,7 +7089,7 @@
         <v>1172290</v>
       </c>
       <c r="X28" s="45" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="Y28" s="9">
         <v>10</v>
@@ -7163,7 +7166,7 @@
         <v>1200000</v>
       </c>
       <c r="X29" s="45" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Y29" s="9">
         <v>10</v>
@@ -7240,7 +7243,7 @@
         <v>1756098</v>
       </c>
       <c r="X30" s="45" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="Y30" s="9">
         <v>10</v>
@@ -7317,7 +7320,7 @@
         <v>1073171</v>
       </c>
       <c r="X31" s="45" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="Y31" s="9">
         <v>10</v>
@@ -7394,7 +7397,7 @@
         <v>65420</v>
       </c>
       <c r="X32" s="45" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="Y32" s="9">
         <v>10</v>
@@ -7471,7 +7474,7 @@
         <v>52495</v>
       </c>
       <c r="X33" s="45" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="Y33" s="9">
         <v>10</v>
@@ -7548,7 +7551,7 @@
         <v>53000</v>
       </c>
       <c r="X34" s="45" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="Y34" s="9">
         <v>10</v>
@@ -7625,7 +7628,7 @@
         <v>63200</v>
       </c>
       <c r="X35" s="45" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="Y35" s="9">
         <v>10</v>
@@ -7702,7 +7705,7 @@
         <v>49275</v>
       </c>
       <c r="X36" s="45" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Y36" s="9">
         <v>10</v>
@@ -7779,7 +7782,7 @@
         <v>45000</v>
       </c>
       <c r="X37" s="45" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="Y37" s="9">
         <v>10</v>
@@ -7856,7 +7859,7 @@
         <v>40000</v>
       </c>
       <c r="X38" s="45" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="Y38" s="9">
         <v>10</v>
@@ -7933,7 +7936,7 @@
         <v>378459</v>
       </c>
       <c r="X39" s="45" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Y39" s="9">
         <v>10</v>
@@ -8011,7 +8014,7 @@
         <v>127550</v>
       </c>
       <c r="X40" s="45" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="Y40" s="9">
         <v>10</v>
@@ -8089,7 +8092,7 @@
         <v>648505</v>
       </c>
       <c r="X41" s="45" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Y41" s="9">
         <v>10</v>
@@ -8167,7 +8170,7 @@
         <v>16801</v>
       </c>
       <c r="X42" s="45" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="Y42" s="9">
         <v>10</v>
@@ -8244,7 +8247,7 @@
         <v>46734</v>
       </c>
       <c r="X43" s="45" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="Y43" s="9">
         <v>10</v>
@@ -8321,7 +8324,7 @@
         <v>90</v>
       </c>
       <c r="X44" s="45" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="Y44" s="9">
         <v>10</v>
@@ -8398,7 +8401,7 @@
         <v>21542</v>
       </c>
       <c r="X45" s="45" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="Y45" s="9">
         <v>10</v>
@@ -8475,7 +8478,7 @@
         <v>16251</v>
       </c>
       <c r="X46" s="45" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Y46" s="9">
         <v>10</v>
@@ -8552,7 +8555,7 @@
         <v>1200000</v>
       </c>
       <c r="X47" s="45" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Y47" s="9">
         <v>10</v>
@@ -8629,7 +8632,7 @@
         <v>0</v>
       </c>
       <c r="X48" s="45" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="Y48" s="9">
         <v>10</v>
@@ -8706,7 +8709,7 @@
         <v>1258848</v>
       </c>
       <c r="X49" s="45" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="Y49" s="9">
         <v>10</v>
@@ -8783,7 +8786,7 @@
         <v>147050</v>
       </c>
       <c r="X50" s="45" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Y50" s="9">
         <v>10</v>
@@ -8860,7 +8863,7 @@
         <v>44295</v>
       </c>
       <c r="X51" s="45" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="Y51" s="9">
         <v>10</v>

</xml_diff>